<commit_message>
2-nd part of lab5 MatProg
</commit_message>
<xml_diff>
--- a/MatProg/Lab5/Lab5.xlsx
+++ b/MatProg/Lab5/Lab5.xlsx
@@ -8,107 +8,183 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\MatProg\Lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0588212A-2658-479A-9922-D5875EBFBEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B90A48-E035-46EC-9B20-193056D7E65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Задание 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Задание 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Задание 1'!$M$24:$N$33,'Задание 1'!$R$24:$R$33</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Задание 2'!$D$7:$E$14,'Задание 2'!$I$7:$I$14</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Задание 1'!$M$24:$M$26</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Задание 2'!$D$10</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Задание 1'!$M$32</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Задание 2'!$D$7:$D$9</definedName>
     <definedName name="solver_lhs11" localSheetId="0" hidden="1">'Задание 1'!$M$32</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Задание 2'!$F$14</definedName>
     <definedName name="solver_lhs12" localSheetId="0" hidden="1">'Задание 1'!$M$32</definedName>
+    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Задание 2'!$F$7:$F$13</definedName>
     <definedName name="solver_lhs13" localSheetId="0" hidden="1">'Задание 1'!$M$33</definedName>
+    <definedName name="solver_lhs13" localSheetId="1" hidden="1">'Задание 2'!$F$7:$F$13</definedName>
     <definedName name="solver_lhs14" localSheetId="0" hidden="1">'Задание 1'!$M$33</definedName>
+    <definedName name="solver_lhs14" localSheetId="1" hidden="1">'Задание 2'!$I$15</definedName>
     <definedName name="solver_lhs15" localSheetId="0" hidden="1">'Задание 1'!$N$30</definedName>
+    <definedName name="solver_lhs15" localSheetId="1" hidden="1">'Задание 2'!$I$7:$I$14</definedName>
     <definedName name="solver_lhs16" localSheetId="0" hidden="1">'Задание 1'!$N$32</definedName>
+    <definedName name="solver_lhs16" localSheetId="1" hidden="1">'Задание 2'!$I$7:$I$14</definedName>
     <definedName name="solver_lhs17" localSheetId="0" hidden="1">'Задание 1'!$N$33</definedName>
     <definedName name="solver_lhs18" localSheetId="0" hidden="1">'Задание 1'!$O$24:$O$33</definedName>
     <definedName name="solver_lhs19" localSheetId="0" hidden="1">'Задание 1'!$O$24:$O$33</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Задание 1'!$M$24:$N$33</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Задание 2'!$D$11</definedName>
     <definedName name="solver_lhs20" localSheetId="0" hidden="1">'Задание 1'!$R$24:$R$33</definedName>
     <definedName name="solver_lhs21" localSheetId="0" hidden="1">'Задание 1'!$R$24:$R$33</definedName>
     <definedName name="solver_lhs22" localSheetId="0" hidden="1">'Задание 1'!$R$24:$R$33</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Задание 1'!$M$27</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Задание 2'!$D$11</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Задание 1'!$M$28</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Задание 2'!$D$12</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Задание 1'!$M$29</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Задание 2'!$D$12</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Задание 1'!$M$30</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Задание 2'!$D$13</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Задание 1'!$M$31</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Задание 2'!$D$13</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Задание 1'!$M$31</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Задание 2'!$D$14</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Задание 1'!$M$31</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Задание 2'!$D$14</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">20</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">14</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Задание 1'!$R$35</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Задание 2'!$I$16</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel11" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel12" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel12" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel13" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel13" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel14" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel14" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel15" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel15" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel16" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel16" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel17" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel18" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel19" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel20" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel21" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel22" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Задание 2'!$E$7</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">'Задание 1'!$N$26</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs11" localSheetId="0" hidden="1">'Задание 1'!$N$27</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs12" localSheetId="0" hidden="1">'Задание 1'!$N$29</definedName>
+    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Задание 2'!$G$7:$G$13</definedName>
     <definedName name="solver_rhs13" localSheetId="0" hidden="1">'Задание 1'!$N$28</definedName>
+    <definedName name="solver_rhs13" localSheetId="1" hidden="1">'Задание 2'!$J$7:$J$13</definedName>
     <definedName name="solver_rhs14" localSheetId="0" hidden="1">'Задание 1'!$N$31</definedName>
+    <definedName name="solver_rhs14" localSheetId="1" hidden="1">'Задание 2'!$I$2</definedName>
     <definedName name="solver_rhs15" localSheetId="0" hidden="1">'Задание 1'!$L$2</definedName>
+    <definedName name="solver_rhs15" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs16" localSheetId="0" hidden="1">'Задание 1'!$L$2</definedName>
+    <definedName name="solver_rhs16" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs17" localSheetId="0" hidden="1">'Задание 1'!$L$2</definedName>
     <definedName name="solver_rhs18" localSheetId="0" hidden="1">'Задание 1'!$P$24:$P$33</definedName>
     <definedName name="solver_rhs19" localSheetId="0" hidden="1">'Задание 1'!$S$24:$S$33</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Задание 2'!$E$10</definedName>
     <definedName name="solver_rhs20" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs21" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs22" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Задание 1'!$N$24</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Задание 2'!$E$8</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Задание 1'!$N$24</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Задание 2'!$E$10</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Задание 1'!$N$25</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Задание 2'!$E$8</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Задание 1'!$N$25</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Задание 2'!$E$11</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">'Задание 1'!$N$26</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Задание 2'!$E$9</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">'Задание 1'!$N$27</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Задание 2'!$E$12</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">'Задание 1'!$N$29</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Задание 2'!$E$13</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -120,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>tij</t>
   </si>
@@ -235,6 +311,27 @@
   <si>
     <t>После оптимизации</t>
   </si>
+  <si>
+    <t>(i, j)</t>
+  </si>
+  <si>
+    <t>(2, 3)</t>
+  </si>
+  <si>
+    <t>(3, 5)</t>
+  </si>
+  <si>
+    <t>tкр</t>
+  </si>
+  <si>
+    <t>xсум</t>
+  </si>
+  <si>
+    <t>До вложения</t>
+  </si>
+  <si>
+    <t>После вложения</t>
+  </si>
 </sst>
 </file>
 
@@ -269,19 +366,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2718,6 +2826,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>601070</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D349672-7A5E-9459-0B17-8B844327F075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6736080" y="236220"/>
+          <a:ext cx="7276190" cy="4076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53341</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>52334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>586741</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>9019</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114D72E0-2F88-6CB7-B551-B96B29E8882D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6758941" y="4624334"/>
+          <a:ext cx="7239000" cy="3980045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2983,16 +3184,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3029,20 +3230,20 @@
       <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3076,28 +3277,21 @@
       <c r="K2" s="1">
         <v>13</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="8">
         <v>40</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3131,26 +3325,19 @@
       <c r="K3" s="1">
         <v>9</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="L3" s="8"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3184,77 +3371,56 @@
       <c r="K4" s="1">
         <v>0.5</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="L4" s="8"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3288,25 +3454,18 @@
       <c r="K7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3348,25 +3507,18 @@
         <f>INDEX($B$22:$C$27,B8,1)-INDEX($B$22:$C$27,A8,1)-C8</f>
         <v>0</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -3408,25 +3560,18 @@
         <f t="shared" ref="K9:K17" si="7">INDEX($B$22:$C$27,B9,1)-INDEX($B$22:$C$27,A9,1)-C9</f>
         <v>0</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -3468,25 +3613,18 @@
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -3528,25 +3666,18 @@
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -3588,25 +3719,18 @@
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -3648,25 +3772,18 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -3708,25 +3825,18 @@
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -3768,25 +3878,18 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -3828,25 +3931,18 @@
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="3"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -3888,68 +3984,47 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
       <c r="E20" s="1" t="s">
         <v>11</v>
       </c>
@@ -3959,27 +4034,20 @@
       <c r="G20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -4001,18 +4069,18 @@
         <f>H8</f>
         <v>14</v>
       </c>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -4034,18 +4102,18 @@
         <f t="shared" ref="G22:G30" si="10">H9</f>
         <v>0</v>
       </c>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -4097,18 +4165,18 @@
       <c r="S23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -4164,18 +4232,18 @@
         <f>B3</f>
         <v>5</v>
       </c>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
-      <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>4</v>
       </c>
@@ -4231,18 +4299,18 @@
         <f>C3</f>
         <v>10</v>
       </c>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="3"/>
-      <c r="AD25" s="3"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>5</v>
       </c>
@@ -4298,18 +4366,18 @@
         <f>D3</f>
         <v>16</v>
       </c>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -4365,18 +4433,18 @@
         <f>E3</f>
         <v>7</v>
       </c>
-      <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
-      <c r="Z27" s="3"/>
-      <c r="AA27" s="3"/>
-      <c r="AB27" s="3"/>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="3"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="7"/>
+      <c r="AD27" s="7"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E28" s="1">
         <f t="shared" si="8"/>
         <v>29</v>
@@ -4423,18 +4491,18 @@
         <f>F3</f>
         <v>11</v>
       </c>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AA28" s="3"/>
-      <c r="AB28" s="3"/>
-      <c r="AC28" s="3"/>
-      <c r="AD28" s="3"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
+      <c r="AB28" s="7"/>
+      <c r="AC28" s="7"/>
+      <c r="AD28" s="7"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E29" s="1">
         <f t="shared" si="8"/>
         <v>29</v>
@@ -4481,18 +4549,18 @@
         <f>G3</f>
         <v>13</v>
       </c>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
+      <c r="AC29" s="7"/>
+      <c r="AD29" s="7"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="E30" s="1">
         <f t="shared" si="8"/>
         <v>39</v>
@@ -4539,18 +4607,18 @@
         <f>H3</f>
         <v>12</v>
       </c>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
-      <c r="AB30" s="3"/>
-      <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J31" s="1">
         <v>4</v>
       </c>
@@ -4585,18 +4653,18 @@
         <f>I3</f>
         <v>7</v>
       </c>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
-      <c r="AB31" s="3"/>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="3"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="J32" s="1">
         <v>4</v>
       </c>
@@ -4631,28 +4699,28 @@
         <f>J3</f>
         <v>15</v>
       </c>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
-      <c r="AA32" s="3"/>
-      <c r="AB32" s="3"/>
-      <c r="AC32" s="3"/>
-      <c r="AD32" s="3"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
       <c r="J33" s="1">
         <v>5</v>
       </c>
@@ -4687,46 +4755,46 @@
         <f>K3</f>
         <v>9</v>
       </c>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
-      <c r="AA33" s="3"/>
-      <c r="AB33" s="3"/>
-      <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
-      <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
       <c r="Q35" s="1" t="s">
         <v>31</v>
       </c>
@@ -4734,122 +4802,122 @@
         <f>SUM(R24:R33)</f>
         <v>116.66666666666819</v>
       </c>
-      <c r="S35" s="5" t="s">
+      <c r="S35" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
-      <c r="W35" s="3"/>
-      <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
-      <c r="Z35" s="3"/>
-      <c r="AA35" s="3"/>
-      <c r="AB35" s="3"/>
-      <c r="AC35" s="3"/>
-      <c r="AD35" s="3"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="3"/>
-      <c r="AA36" s="3"/>
-      <c r="AB36" s="3"/>
-      <c r="AC36" s="3"/>
-      <c r="AD36" s="3"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-      <c r="Z37" s="3"/>
-      <c r="AA37" s="3"/>
-      <c r="AB37" s="3"/>
-      <c r="AC37" s="3"/>
-      <c r="AD37" s="3"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="3"/>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="3"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="J40" s="3" t="s">
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="J40" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
       <c r="J41" s="1" t="s">
         <v>5</v>
       </c>
@@ -4884,15 +4952,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
       <c r="J42" s="1">
         <v>1</v>
       </c>
@@ -4936,15 +5004,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
       <c r="J43" s="1">
         <v>1</v>
       </c>
@@ -4988,15 +5056,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
       <c r="J44" s="1">
         <v>1</v>
       </c>
@@ -5040,15 +5108,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
       <c r="J45" s="1">
         <v>2</v>
       </c>
@@ -5092,15 +5160,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
       <c r="J46" s="1">
         <v>2</v>
       </c>
@@ -5144,15 +5212,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
       <c r="J47" s="1">
         <v>3</v>
       </c>
@@ -5196,15 +5264,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
       <c r="J48" s="1">
         <v>3</v>
       </c>
@@ -5248,17 +5316,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
       <c r="J49" s="1">
         <v>4</v>
       </c>
@@ -5302,15 +5370,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
       <c r="J50" s="1">
         <v>4</v>
       </c>
@@ -5354,15 +5422,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
       <c r="J51" s="1">
         <v>5</v>
       </c>
@@ -5406,30 +5474,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="J53" s="3" t="s">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="J53" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
       <c r="N53" s="1" t="s">
         <v>11</v>
       </c>
@@ -5440,15 +5508,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
       <c r="J54" s="1" t="s">
         <v>5</v>
       </c>
@@ -5471,15 +5539,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
       <c r="J55" s="1">
         <v>1</v>
       </c>
@@ -5502,15 +5570,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
       <c r="J56" s="1">
         <v>2</v>
       </c>
@@ -5533,15 +5601,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
       <c r="J57" s="1">
         <v>3</v>
       </c>
@@ -5564,15 +5632,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
       <c r="J58" s="1">
         <v>4</v>
       </c>
@@ -5595,15 +5663,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
       <c r="J59" s="1">
         <v>5</v>
       </c>
@@ -5626,15 +5694,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
       <c r="J60" s="1">
         <v>6</v>
       </c>
@@ -5657,15 +5725,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
       <c r="N61" s="1">
         <f t="shared" si="22"/>
         <v>23</v>
@@ -5679,15 +5747,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
       <c r="N62" s="1">
         <f t="shared" si="22"/>
         <v>23</v>
@@ -5701,15 +5769,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
       <c r="N63" s="1">
         <f t="shared" si="22"/>
         <v>31</v>
@@ -5723,15 +5791,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -5755,4 +5823,1209 @@
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB8135E-0155-40F5-9102-0B8BACC02C60}">
+  <dimension ref="A1:W48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
+        <v>7</v>
+      </c>
+      <c r="I2" s="8">
+        <v>47</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ref="F7:F14" si="0">E7-D7</f>
+        <v>12</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ref="G7:G14" si="1">C7-H7*I7</f>
+        <v>12</v>
+      </c>
+      <c r="H7" s="1">
+        <f>B4</f>
+        <v>0.25</v>
+      </c>
+      <c r="I7" s="1">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1">
+        <f>B3</f>
+        <v>12</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H8" s="1">
+        <f>C4</f>
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f>C3</f>
+        <v>5</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H9" s="1">
+        <f>D4</f>
+        <v>0.15</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <f>D3</f>
+        <v>4</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999964</v>
+      </c>
+      <c r="H10" s="1">
+        <f>E4</f>
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>10.000000000000036</v>
+      </c>
+      <c r="J10" s="1">
+        <f>E3</f>
+        <v>3</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>10.000000000000007</v>
+      </c>
+      <c r="H11" s="1">
+        <f>F4</f>
+        <v>0.3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>9.9999999999999769</v>
+      </c>
+      <c r="J11" s="1">
+        <f>F3</f>
+        <v>10</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H12" s="1">
+        <f>G4</f>
+        <v>0.4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <f>G3</f>
+        <v>8</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1">
+        <v>30</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000027</v>
+      </c>
+      <c r="H13" s="1">
+        <f>H4</f>
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>14.999999999999986</v>
+      </c>
+      <c r="J13" s="1">
+        <f>H3</f>
+        <v>4</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>30</v>
+      </c>
+      <c r="E14" s="1">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1">
+        <f>SUM(I7:I14)</f>
+        <v>47</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="1">
+        <f>E14</f>
+        <v>30</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+    </row>
+    <row r="18" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+    </row>
+    <row r="19" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+      <c r="D20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+    </row>
+    <row r="21" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+      <c r="D21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+    </row>
+    <row r="22" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+      <c r="D22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C23" s="2"/>
+      <c r="D23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+    </row>
+    <row r="24" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C24" s="2"/>
+      <c r="D24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+    </row>
+    <row r="25" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+      <c r="D25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+    </row>
+    <row r="26" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C26" s="2"/>
+      <c r="D26" s="4"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+    </row>
+    <row r="27" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C27" s="2"/>
+      <c r="D27" s="4"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+    </row>
+    <row r="28" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
+      <c r="D28" s="4"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+    </row>
+    <row r="29" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C29" s="2"/>
+      <c r="D29" s="4"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+    </row>
+    <row r="30" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+    </row>
+    <row r="31" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+    </row>
+    <row r="32" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+    </row>
+    <row r="33" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+    </row>
+    <row r="34" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+    </row>
+    <row r="35" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+    </row>
+    <row r="36" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+    </row>
+    <row r="37" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+    </row>
+    <row r="38" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+    </row>
+    <row r="39" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+    </row>
+    <row r="40" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+    </row>
+    <row r="41" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+    </row>
+    <row r="42" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7"/>
+      <c r="W42" s="7"/>
+    </row>
+    <row r="43" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
+      <c r="W43" s="7"/>
+    </row>
+    <row r="44" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+    </row>
+    <row r="45" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+    </row>
+    <row r="46" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+    </row>
+    <row r="47" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+    </row>
+    <row r="48" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="L26:W48"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="L2:W24"/>
+    <mergeCell ref="L1:W1"/>
+    <mergeCell ref="L25:W25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All final fixes in labs MatProg
</commit_message>
<xml_diff>
--- a/MatProg/Lab5/Lab5.xlsx
+++ b/MatProg/Lab5/Lab5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\MatProg\Lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B90A48-E035-46EC-9B20-193056D7E65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802509FA-867C-4856-802A-11FD540604DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Задание 1" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
   <si>
     <t>tij</t>
   </si>
@@ -304,12 +304,6 @@
   </si>
   <si>
     <t>-&gt; min</t>
-  </si>
-  <si>
-    <t>До оптимизации</t>
-  </si>
-  <si>
-    <t>После оптимизации</t>
   </si>
   <si>
     <t>(i, j)</t>
@@ -3184,8 +3178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3231,7 +3225,7 @@
         <v>3</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V1" s="7"/>
       <c r="W1" s="7"/>
@@ -4035,7 +4029,7 @@
         <v>15</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
@@ -4712,7 +4706,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -5318,7 +5312,7 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -5829,7 +5823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB8135E-0155-40F5-9102-0B8BACC02C60}">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -5837,7 +5831,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
@@ -5849,22 +5843,22 @@
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -6473,7 +6467,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I16" s="1">
         <f>E14</f>
@@ -6673,7 +6667,7 @@
       <c r="J25" s="5"/>
       <c r="K25" s="1"/>
       <c r="L25" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>

</xml_diff>